<commit_message>
some more res and stats
</commit_message>
<xml_diff>
--- a/Proj/src/res/DependencyParts.xlsx
+++ b/Proj/src/res/DependencyParts.xlsx
@@ -9,17 +9,17 @@
   <sheets>
     <sheet name="dependency parts" sheetId="1" r:id="rId1"/>
     <sheet name="20.01.2015 data" sheetId="2" r:id="rId2"/>
-    <sheet name="16.02.2015" sheetId="3" r:id="rId3"/>
+    <sheet name="17.02.2015" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'16.02.2015'!$A$1:$K$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'17.02.2015'!$A$1:$K$13</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="79">
   <si>
     <t>part name</t>
   </si>
@@ -253,14 +253,25 @@
   </si>
   <si>
     <t>gold</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -288,7 +299,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -620,16 +631,40 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -670,126 +705,94 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1925,11 +1928,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1978,458 +1980,737 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="30">
         <v>0.83407008685716399</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="31">
         <v>0.99621644843864898</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="31">
         <v>0.83358619641756004</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="31">
         <v>0.93997884084703498</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="31">
         <v>0.88171398810639401</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="31">
         <v>0.88106052107069699</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="33">
         <v>0.834256673859326</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="34">
         <v>0.99641301139875305</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="34">
         <v>0.83358619641756004</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="34">
         <v>0.93997884084703498</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="34">
         <v>0.88190556308752599</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="34">
         <v>0.88106052107069699</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="33">
         <v>0.83400704747751397</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="34">
         <v>0.99696552564210394</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="34">
         <v>0.83450492584264901</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="34">
         <v>0.93997884084703498</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="34">
         <v>0.88221612702960595</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="34">
         <v>0.88269300337802303</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="33">
         <v>0.83418878802730001</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="34">
         <v>0.99714823160717503</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="34">
         <v>0.83450492584264901</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="34">
         <v>0.93997884084703498</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="34">
         <v>0.88240784353733304</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="34">
         <v>0.88269300337802303</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
         <v>0.86703941206899005</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="34">
         <v>0.92583440314753496</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="34">
         <v>0.90244491626616896</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="34">
         <v>0.93997884084703498</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="34">
         <v>0.89572596432735696</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="34">
         <v>0.94646923433036301</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="33">
         <v>0.87424221104059996</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="34">
         <v>0.93927663372151404</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="34">
         <v>0.90244491626616896</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="34">
         <v>0.93997884084703498</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="34">
         <v>0.90252916235224501</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="34">
         <v>0.94646923433036301</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="33">
         <v>0.88350675084477504</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="34">
         <v>0.93005447658403695</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="34">
         <v>0.91680775982987395</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="34">
         <v>0.93997884084703498</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="34">
         <v>0.91488420028180095</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="34">
         <v>0.96513200738621496</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="35" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="33">
         <v>0.88673644040772504</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="34">
         <v>0.93724412779130595</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="34">
         <v>0.91680775982987395</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="34">
         <v>0.93997884084703498</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="34">
         <v>0.91691364435112599</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="34">
         <v>0.96513200738621496</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="33">
         <v>0.86719983083410901</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="34">
         <v>0.92155189976538998</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="34">
         <v>0.92141052943956703</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="34">
         <v>0.93997884084703498</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="34">
         <v>0.89553611648631004</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="34">
         <v>0.92534985142235904</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="33">
         <v>0.874364285756699</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="34">
         <v>0.93435929532399797</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="34">
         <v>0.92141052943956703</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="34">
         <v>0.93997884084703498</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="34">
         <v>0.90237765856021901</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="34">
         <v>0.92534985142235904</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="33">
         <v>0.88381568808821798</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="34">
         <v>0.92449903590258697</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="34">
         <v>0.94053725308198399</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="34">
         <v>0.93997884084703498</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="34">
         <v>0.91452378605839202</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="34">
         <v>0.93958368730617503</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="39">
         <v>0.88703172312809098</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="40">
         <v>0.93081273422744704</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="40">
         <v>0.94053725308198399</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="40">
         <v>0.93997884084703498</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="40">
         <v>0.916512729258391</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="40">
         <v>0.93958368730617503</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="41" t="s">
         <v>75</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="30">
+        <v>0.86815739440413497</v>
+      </c>
+      <c r="B14" s="31">
+        <v>0.92302575610531601</v>
+      </c>
+      <c r="C14" s="31">
+        <v>0.92191202079752299</v>
+      </c>
+      <c r="D14" s="31">
+        <v>0.93796849734370902</v>
+      </c>
+      <c r="E14" s="31">
+        <v>0.89719468162250404</v>
+      </c>
+      <c r="F14" s="31">
+        <v>0.92516727978792201</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" s="32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="33">
+        <v>0.87513458010095901</v>
+      </c>
+      <c r="B15" s="34">
+        <v>0.93735178348908799</v>
+      </c>
+      <c r="C15" s="34">
+        <v>0.92191202079752299</v>
+      </c>
+      <c r="D15" s="34">
+        <v>0.93796849734370902</v>
+      </c>
+      <c r="E15" s="34">
+        <v>0.90387869794351805</v>
+      </c>
+      <c r="F15" s="34">
+        <v>0.92516727978792201</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" s="35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="33">
+        <v>0.86800843516675497</v>
+      </c>
+      <c r="B16" s="34">
+        <v>0.92660398148304102</v>
+      </c>
+      <c r="C16" s="34">
+        <v>0.90075518880183303</v>
+      </c>
+      <c r="D16" s="34">
+        <v>0.93796849734370902</v>
+      </c>
+      <c r="E16" s="34">
+        <v>0.89731028158044501</v>
+      </c>
+      <c r="F16" s="34">
+        <v>0.94663196855708098</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="K16" s="35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="33">
+        <v>0.87505108183057401</v>
+      </c>
+      <c r="B17" s="34">
+        <v>0.94132929006533494</v>
+      </c>
+      <c r="C17" s="34">
+        <v>0.90075518880183303</v>
+      </c>
+      <c r="D17" s="34">
+        <v>0.93796849734370902</v>
+      </c>
+      <c r="E17" s="34">
+        <v>0.90399049203128401</v>
+      </c>
+      <c r="F17" s="34">
+        <v>0.94663196855708098</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="K17" s="35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="33">
+        <v>0.88442313378623405</v>
+      </c>
+      <c r="B18" s="34">
+        <v>0.92466951267559105</v>
+      </c>
+      <c r="C18" s="34">
+        <v>0.93948676299548395</v>
+      </c>
+      <c r="D18" s="34">
+        <v>0.93796849734370902</v>
+      </c>
+      <c r="E18" s="34">
+        <v>0.91378312996564304</v>
+      </c>
+      <c r="F18" s="34">
+        <v>0.93749634803878701</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" s="35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="42">
+        <v>0.88779589760050803</v>
+      </c>
+      <c r="B19" s="43">
+        <v>0.93259163628542097</v>
+      </c>
+      <c r="C19" s="43">
+        <v>0.93948676299548395</v>
+      </c>
+      <c r="D19" s="43">
+        <v>0.93796849734370902</v>
+      </c>
+      <c r="E19" s="43">
+        <v>0.91631889255854104</v>
+      </c>
+      <c r="F19" s="43">
+        <v>0.93749634803878701</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="J19" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="33">
+        <v>0.884041293593959</v>
+      </c>
+      <c r="B20" s="34">
+        <v>0.928765908193252</v>
+      </c>
+      <c r="C20" s="34">
+        <v>0.91326245767588698</v>
+      </c>
+      <c r="D20" s="34">
+        <v>0.93796849734370902</v>
+      </c>
+      <c r="E20" s="34">
+        <v>0.914312414379441</v>
+      </c>
+      <c r="F20" s="34">
+        <v>0.96344962023074698</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="J20" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="K20" s="35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="36">
+        <v>0.88737803461248799</v>
+      </c>
+      <c r="B21" s="37">
+        <v>0.93679907705462995</v>
+      </c>
+      <c r="C21" s="37">
+        <v>0.91326245767588698</v>
+      </c>
+      <c r="D21" s="37">
+        <v>0.93796849734370902</v>
+      </c>
+      <c r="E21" s="37">
+        <v>0.91680140054320802</v>
+      </c>
+      <c r="F21" s="37">
+        <v>0.96344962023074698</v>
+      </c>
+      <c r="G21" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="J21" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="K21" s="38" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K13">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="proj"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="8">
-      <filters>
-        <filter val="noNegW"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="10">
-      <filters>
-        <filter val="allSlack"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K13"/>
   <conditionalFormatting sqref="A2:A13">
-    <cfRule type="top10" dxfId="19" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="10" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B13">
-    <cfRule type="top10" dxfId="11" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="9" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="8" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="top10" dxfId="4" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="7" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
-    <cfRule type="top10" dxfId="1" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="6" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:A21">
+    <cfRule type="top10" dxfId="4" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:B21">
+    <cfRule type="top10" dxfId="3" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:C21">
+    <cfRule type="top10" dxfId="2" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E21">
+    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14:F21">
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changing uas calculations, adding alpha to objective functino
</commit_message>
<xml_diff>
--- a/Proj/src/res/DependencyParts.xlsx
+++ b/Proj/src/res/DependencyParts.xlsx
@@ -12,14 +12,14 @@
     <sheet name="17.02.2015" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'17.02.2015'!$A$1:$K$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'17.02.2015'!$A$1:$L$13</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="80">
   <si>
     <t>part name</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>alpha</t>
   </si>
 </sst>
 </file>
@@ -1928,10 +1931,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,12 +1943,12 @@
     <col min="4" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="8" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>48</v>
       </c>
@@ -1974,13 +1977,16 @@
         <v>68</v>
       </c>
       <c r="J1" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="L1" s="29" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="30">
         <v>0.83407008685716399</v>
       </c>
@@ -2008,14 +2014,17 @@
       <c r="I2" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="31">
+        <v>1</v>
+      </c>
+      <c r="K2" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="L2" s="32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="33">
         <v>0.834256673859326</v>
       </c>
@@ -2043,14 +2052,17 @@
       <c r="I3" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="J3" s="34" t="s">
+      <c r="J3" s="34">
+        <v>1</v>
+      </c>
+      <c r="K3" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K3" s="35" t="s">
+      <c r="L3" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="33">
         <v>0.83400704747751397</v>
       </c>
@@ -2078,14 +2090,17 @@
       <c r="I4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="J4" s="34" t="s">
+      <c r="J4" s="34">
+        <v>1</v>
+      </c>
+      <c r="K4" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="L4" s="35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="33">
         <v>0.83418878802730001</v>
       </c>
@@ -2113,14 +2128,17 @@
       <c r="I5" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="J5" s="34" t="s">
+      <c r="J5" s="34">
+        <v>1</v>
+      </c>
+      <c r="K5" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K5" s="35" t="s">
+      <c r="L5" s="35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="33">
         <v>0.86703941206899005</v>
       </c>
@@ -2148,14 +2166,17 @@
       <c r="I6" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="34">
+        <v>1</v>
+      </c>
+      <c r="K6" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K6" s="35" t="s">
+      <c r="L6" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
         <v>0.87424221104059996</v>
       </c>
@@ -2183,14 +2204,17 @@
       <c r="I7" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J7" s="34">
+        <v>1</v>
+      </c>
+      <c r="K7" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K7" s="35" t="s">
+      <c r="L7" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
         <v>0.88350675084477504</v>
       </c>
@@ -2218,14 +2242,17 @@
       <c r="I8" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="J8" s="34">
+        <v>1</v>
+      </c>
+      <c r="K8" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K8" s="35" t="s">
+      <c r="L8" s="35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="33">
         <v>0.88673644040772504</v>
       </c>
@@ -2253,14 +2280,17 @@
       <c r="I9" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J9" s="34" t="s">
+      <c r="J9" s="34">
+        <v>1</v>
+      </c>
+      <c r="K9" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K9" s="35" t="s">
+      <c r="L9" s="35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="33">
         <v>0.86719983083410901</v>
       </c>
@@ -2288,14 +2318,17 @@
       <c r="I10" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="34" t="s">
+      <c r="J10" s="34">
+        <v>1</v>
+      </c>
+      <c r="K10" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="K10" s="35" t="s">
+      <c r="L10" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="33">
         <v>0.874364285756699</v>
       </c>
@@ -2323,14 +2356,17 @@
       <c r="I11" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J11" s="34" t="s">
+      <c r="J11" s="34">
+        <v>1</v>
+      </c>
+      <c r="K11" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="K11" s="35" t="s">
+      <c r="L11" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="33">
         <v>0.88381568808821798</v>
       </c>
@@ -2358,14 +2394,17 @@
       <c r="I12" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="34" t="s">
+      <c r="J12" s="34">
+        <v>1</v>
+      </c>
+      <c r="K12" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="K12" s="35" t="s">
+      <c r="L12" s="35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="39">
         <v>0.88703172312809098</v>
       </c>
@@ -2393,14 +2432,17 @@
       <c r="I13" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="J13" s="40" t="s">
+      <c r="J13" s="40">
+        <v>1</v>
+      </c>
+      <c r="K13" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="K13" s="41" t="s">
+      <c r="L13" s="41" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
         <v>0.86815739440413497</v>
       </c>
@@ -2428,14 +2470,17 @@
       <c r="I14" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="J14" s="31" t="s">
+      <c r="J14" s="31">
+        <v>1</v>
+      </c>
+      <c r="K14" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="K14" s="32" t="s">
+      <c r="L14" s="32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="33">
         <v>0.87513458010095901</v>
       </c>
@@ -2463,14 +2508,17 @@
       <c r="I15" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J15" s="34" t="s">
+      <c r="J15" s="34">
+        <v>1</v>
+      </c>
+      <c r="K15" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="K15" s="35" t="s">
+      <c r="L15" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="33">
         <v>0.86800843516675497</v>
       </c>
@@ -2498,14 +2546,17 @@
       <c r="I16" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J16" s="34" t="s">
+      <c r="J16" s="34">
+        <v>1</v>
+      </c>
+      <c r="K16" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K16" s="35" t="s">
+      <c r="L16" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="33">
         <v>0.87505108183057401</v>
       </c>
@@ -2533,14 +2584,17 @@
       <c r="I17" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J17" s="34" t="s">
+      <c r="J17" s="34">
+        <v>1</v>
+      </c>
+      <c r="K17" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K17" s="35" t="s">
+      <c r="L17" s="35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="33">
         <v>0.88442313378623405</v>
       </c>
@@ -2568,14 +2622,17 @@
       <c r="I18" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J18" s="34" t="s">
+      <c r="J18" s="34">
+        <v>1</v>
+      </c>
+      <c r="K18" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="K18" s="35" t="s">
+      <c r="L18" s="35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="42">
         <v>0.88779589760050803</v>
       </c>
@@ -2603,14 +2660,17 @@
       <c r="I19" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="J19" s="43" t="s">
+      <c r="J19" s="43">
+        <v>1</v>
+      </c>
+      <c r="K19" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="K19" s="44" t="s">
+      <c r="L19" s="44" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="33">
         <v>0.884041293593959</v>
       </c>
@@ -2638,14 +2698,17 @@
       <c r="I20" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="J20" s="34" t="s">
+      <c r="J20" s="34">
+        <v>1</v>
+      </c>
+      <c r="K20" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K20" s="35" t="s">
+      <c r="L20" s="35" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="36">
         <v>0.88737803461248799</v>
       </c>
@@ -2673,15 +2736,18 @@
       <c r="I21" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="J21" s="37" t="s">
+      <c r="J21" s="37">
+        <v>1</v>
+      </c>
+      <c r="K21" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="K21" s="38" t="s">
+      <c r="L21" s="38" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K13"/>
+  <autoFilter ref="A1:L13"/>
   <conditionalFormatting sqref="A2:A13">
     <cfRule type="top10" dxfId="9" priority="10" rank="1"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
bug fix and data update
</commit_message>
<xml_diff>
--- a/Proj/src/res/DependencyParts.xlsx
+++ b/Proj/src/res/DependencyParts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3"/>
@@ -11,16 +11,17 @@
     <sheet name="20.01.2015 data" sheetId="2" r:id="rId2"/>
     <sheet name="17.02.2015" sheetId="3" r:id="rId3"/>
     <sheet name="19.02.2015" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'17.02.2015'!$A$1:$L$13</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="85">
   <si>
     <t>part name</t>
   </si>
@@ -269,17 +270,23 @@
   </si>
   <si>
     <t>non projective lp formulation</t>
+  </si>
+  <si>
+    <t>projective ILP formulation</t>
+  </si>
+  <si>
+    <t>projInference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -287,7 +294,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -875,231 +882,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <fill>
         <patternFill>
@@ -1373,7 +1156,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1405,10 +1188,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1440,7 +1222,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1616,22 +1397,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1645,7 +1426,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
@@ -1655,7 +1436,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
@@ -1667,7 +1448,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="15" t="s">
         <v>7</v>
       </c>
@@ -1679,7 +1460,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
@@ -1693,7 +1474,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="15" t="s">
         <v>11</v>
       </c>
@@ -1707,7 +1488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="15" t="s">
         <v>12</v>
       </c>
@@ -1721,7 +1502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
@@ -1731,7 +1512,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="15" t="s">
         <v>16</v>
       </c>
@@ -1745,7 +1526,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="15" t="s">
         <v>18</v>
       </c>
@@ -1757,7 +1538,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="15" t="s">
         <v>20</v>
       </c>
@@ -1771,7 +1552,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="15" t="s">
         <v>21</v>
       </c>
@@ -1785,7 +1566,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="15" t="s">
         <v>22</v>
       </c>
@@ -1799,7 +1580,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="15" t="s">
         <v>23</v>
       </c>
@@ -1811,7 +1592,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="15" t="s">
         <v>25</v>
       </c>
@@ -1825,7 +1606,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="15" t="s">
         <v>28</v>
       </c>
@@ -1839,7 +1620,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="15" t="s">
         <v>29</v>
       </c>
@@ -1853,7 +1634,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15" thickBot="1">
       <c r="A18" s="16" t="s">
         <v>31</v>
       </c>
@@ -1871,29 +1652,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.75" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" style="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.25" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.125" customWidth="1"/>
+    <col min="8" max="8" width="19.25" customWidth="1"/>
+    <col min="9" max="9" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" thickBot="1"/>
+    <row r="3" spans="1:10" ht="29.25" thickBot="1">
       <c r="A3" s="24" t="s">
         <v>56</v>
       </c>
@@ -1922,7 +1703,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="24" t="s">
         <v>58</v>
       </c>
@@ -1951,7 +1732,7 @@
         <v>77.7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15" thickBot="1">
       <c r="A5" s="24" t="s">
         <v>59</v>
       </c>
@@ -1980,7 +1761,7 @@
         <v>87.76</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15" thickBot="1">
       <c r="A6" s="24" t="s">
         <v>62</v>
       </c>
@@ -1988,7 +1769,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="29.25" thickBot="1">
       <c r="C7" s="23" t="s">
         <v>55</v>
       </c>
@@ -2011,7 +1792,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="C8" s="18" t="s">
         <v>46</v>
       </c>
@@ -2034,7 +1815,7 @@
         <v>77.7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15" thickBot="1">
       <c r="C9" s="16" t="s">
         <v>47</v>
       </c>
@@ -2057,7 +1838,7 @@
         <v>87.76</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="C10" s="25"/>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
@@ -2067,7 +1848,7 @@
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15" thickBot="1">
       <c r="C11" s="25"/>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
@@ -2077,7 +1858,7 @@
       <c r="I11" s="26"/>
       <c r="J11" s="26"/>
     </row>
-    <row r="12" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="29.25" thickBot="1">
       <c r="A12" s="24" t="s">
         <v>56</v>
       </c>
@@ -2106,7 +1887,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="24" t="s">
         <v>58</v>
       </c>
@@ -2135,7 +1916,7 @@
         <v>83.45</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="15" thickBot="1">
       <c r="A14" s="24" t="s">
         <v>59</v>
       </c>
@@ -2164,7 +1945,7 @@
         <v>83.63</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" thickBot="1">
       <c r="A15" s="24" t="s">
         <v>62</v>
       </c>
@@ -2172,7 +1953,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="29.25" thickBot="1">
       <c r="C16" s="23" t="s">
         <v>55</v>
       </c>
@@ -2195,7 +1976,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="C17" s="18" t="s">
         <v>46</v>
       </c>
@@ -2218,7 +1999,7 @@
         <v>83.45</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15" thickBot="1">
       <c r="C18" s="16" t="s">
         <v>47</v>
       </c>
@@ -2241,8 +2022,8 @@
         <v>83.63</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15" thickBot="1"/>
+    <row r="21" spans="1:9" ht="29.25" thickBot="1">
       <c r="A21" s="24" t="s">
         <v>56</v>
       </c>
@@ -2271,7 +2052,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="24" t="s">
         <v>58</v>
       </c>
@@ -2300,7 +2081,7 @@
         <v>74.27</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15" thickBot="1">
       <c r="A23" s="24" t="s">
         <v>59</v>
       </c>
@@ -2329,7 +2110,7 @@
         <v>78.77</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15" thickBot="1">
       <c r="A24" s="24" t="s">
         <v>62</v>
       </c>
@@ -2337,7 +2118,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="29.25" thickBot="1">
       <c r="C25" s="23" t="s">
         <v>55</v>
       </c>
@@ -2360,7 +2141,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="C26" s="18" t="s">
         <v>46</v>
       </c>
@@ -2383,7 +2164,7 @@
         <v>74.27</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15" thickBot="1">
       <c r="C27" s="16" t="s">
         <v>47</v>
       </c>
@@ -2413,25 +2194,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="10.42578125" customWidth="1"/>
+    <col min="1" max="2" width="10.375" customWidth="1"/>
     <col min="4" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.125" customWidth="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1"/>
     <col min="8" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.375" customWidth="1"/>
+    <col min="12" max="12" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="30.75" customHeight="1" thickBot="1">
       <c r="A1" s="27" t="s">
         <v>48</v>
       </c>
@@ -2469,7 +2250,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="30">
         <v>0.83407008685716399</v>
       </c>
@@ -2507,7 +2288,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="33">
         <v>0.834256673859326</v>
       </c>
@@ -2545,7 +2326,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="33">
         <v>0.83400704747751397</v>
       </c>
@@ -2583,7 +2364,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="33">
         <v>0.83418878802730001</v>
       </c>
@@ -2621,7 +2402,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="33">
         <v>0.86703941206899005</v>
       </c>
@@ -2659,7 +2440,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="33">
         <v>0.87424221104059996</v>
       </c>
@@ -2697,7 +2478,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="33">
         <v>0.88350675084477504</v>
       </c>
@@ -2735,7 +2516,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="33">
         <v>0.88673644040772504</v>
       </c>
@@ -2773,7 +2554,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="33">
         <v>0.86719983083410901</v>
       </c>
@@ -2811,7 +2592,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="33">
         <v>0.874364285756699</v>
       </c>
@@ -2849,7 +2630,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="33">
         <v>0.88381568808821798</v>
       </c>
@@ -2887,7 +2668,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15.75" thickBot="1">
       <c r="A13" s="39">
         <v>0.88703172312809098</v>
       </c>
@@ -2925,7 +2706,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="30">
         <v>0.86815739440413497</v>
       </c>
@@ -2963,7 +2744,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="33">
         <v>0.87513458010095901</v>
       </c>
@@ -3001,7 +2782,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="33">
         <v>0.86800843516675497</v>
       </c>
@@ -3039,7 +2820,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="33">
         <v>0.87505108183057401</v>
       </c>
@@ -3077,7 +2858,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="33">
         <v>0.88442313378623405</v>
       </c>
@@ -3115,7 +2896,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15">
       <c r="A19" s="42">
         <v>0.88779589760050803</v>
       </c>
@@ -3153,7 +2934,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="33">
         <v>0.884041293593959</v>
       </c>
@@ -3191,7 +2972,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="15" thickBot="1">
       <c r="A21" s="36">
         <v>0.88737803461248799</v>
       </c>
@@ -3232,34 +3013,34 @@
   </sheetData>
   <autoFilter ref="A1:L13"/>
   <conditionalFormatting sqref="A2:A13">
-    <cfRule type="top10" dxfId="62" priority="10" rank="1"/>
+    <cfRule type="top10" dxfId="30" priority="10" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B13">
-    <cfRule type="top10" dxfId="61" priority="9" rank="1"/>
+    <cfRule type="top10" dxfId="29" priority="9" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C13">
-    <cfRule type="top10" dxfId="60" priority="8" rank="1"/>
+    <cfRule type="top10" dxfId="28" priority="8" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E13">
-    <cfRule type="top10" dxfId="59" priority="7" rank="1"/>
+    <cfRule type="top10" dxfId="27" priority="7" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
-    <cfRule type="top10" dxfId="58" priority="6" rank="1"/>
+    <cfRule type="top10" dxfId="26" priority="6" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A21">
-    <cfRule type="top10" dxfId="57" priority="5" rank="1"/>
+    <cfRule type="top10" dxfId="25" priority="5" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B21">
-    <cfRule type="top10" dxfId="56" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="24" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="top10" dxfId="55" priority="3" rank="1"/>
+    <cfRule type="top10" dxfId="23" priority="3" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:E21">
-    <cfRule type="top10" dxfId="54" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="22" priority="2" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F21">
-    <cfRule type="top10" dxfId="53" priority="1" rank="1"/>
+    <cfRule type="top10" dxfId="21" priority="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3267,27 +3048,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:V34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.875" customWidth="1"/>
+    <col min="4" max="4" width="10.25" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.125" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.875" customWidth="1"/>
+    <col min="11" max="11" width="14.75" customWidth="1"/>
+    <col min="15" max="15" width="10.5" customWidth="1"/>
+    <col min="17" max="17" width="14.625" customWidth="1"/>
+    <col min="21" max="21" width="13.25" customWidth="1"/>
+    <col min="22" max="22" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="37.5" customHeight="1" thickBot="1">
       <c r="A1" s="27" t="s">
         <v>48</v>
       </c>
@@ -3318,8 +3103,41 @@
       <c r="J1" s="29" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="V1" s="27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" s="30">
         <v>0.87183070473148305</v>
       </c>
@@ -3353,8 +3171,41 @@
       <c r="K2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>0.87200539029746404</v>
+      </c>
+      <c r="M2">
+        <v>0.98053503693351896</v>
+      </c>
+      <c r="N2">
+        <v>0.87088241165901303</v>
+      </c>
+      <c r="O2">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P2">
+        <v>0.90669295268516603</v>
+      </c>
+      <c r="Q2">
+        <v>0.90464663605509998</v>
+      </c>
+      <c r="R2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>77</v>
+      </c>
+      <c r="V2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" s="33">
         <v>0.87542423637452504</v>
       </c>
@@ -3385,8 +3236,41 @@
       <c r="J3" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>0.87422639249351097</v>
+      </c>
+      <c r="M3">
+        <v>0.99565781593132296</v>
+      </c>
+      <c r="N3">
+        <v>0.87088241165901303</v>
+      </c>
+      <c r="O3">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P3">
+        <v>0.90816530245557903</v>
+      </c>
+      <c r="Q3">
+        <v>0.90464663605509998</v>
+      </c>
+      <c r="R3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>77</v>
+      </c>
+      <c r="V3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" s="33">
         <v>0.87357756039129497</v>
       </c>
@@ -3417,8 +3301,41 @@
       <c r="J4" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>0.87452585346376499</v>
+      </c>
+      <c r="M4">
+        <v>0.91485326412457502</v>
+      </c>
+      <c r="N4">
+        <v>0.94599720503094398</v>
+      </c>
+      <c r="O4">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P4">
+        <v>0.90831503294070604</v>
+      </c>
+      <c r="Q4">
+        <v>0.93738770213615497</v>
+      </c>
+      <c r="R4" t="s">
+        <v>70</v>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
+        <v>77</v>
+      </c>
+      <c r="V4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="33">
         <v>0.87737073268117305</v>
       </c>
@@ -3449,8 +3366,41 @@
       <c r="J5" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>0.877121181872629</v>
+      </c>
+      <c r="M5">
+        <v>0.92071770812537401</v>
+      </c>
+      <c r="N5">
+        <v>0.94599720503094398</v>
+      </c>
+      <c r="O5">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P5">
+        <v>0.910161708923936</v>
+      </c>
+      <c r="Q5">
+        <v>0.93738770213615497</v>
+      </c>
+      <c r="R5" t="s">
+        <v>84</v>
+      </c>
+      <c r="S5" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="33">
         <v>0.873702335795568</v>
       </c>
@@ -3481,8 +3431,41 @@
       <c r="J6" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>0.87452585346376499</v>
+      </c>
+      <c r="M6">
+        <v>0.88128868037532404</v>
+      </c>
+      <c r="N6">
+        <v>0.98697344779397</v>
+      </c>
+      <c r="O6">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P6">
+        <v>0.90831503294070604</v>
+      </c>
+      <c r="Q6">
+        <v>0.93399381113994795</v>
+      </c>
+      <c r="R6" t="s">
+        <v>70</v>
+      </c>
+      <c r="S6" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>3</v>
+      </c>
+      <c r="U6" t="s">
+        <v>77</v>
+      </c>
+      <c r="V6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="33">
         <v>0.877445597923737</v>
       </c>
@@ -3513,8 +3496,41 @@
       <c r="J7" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>0.87714613695348298</v>
+      </c>
+      <c r="M7">
+        <v>0.88620483130365302</v>
+      </c>
+      <c r="N7">
+        <v>0.98697344779397</v>
+      </c>
+      <c r="O7">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P7">
+        <v>0.91018666400479098</v>
+      </c>
+      <c r="Q7">
+        <v>0.93399381113994795</v>
+      </c>
+      <c r="R7" t="s">
+        <v>84</v>
+      </c>
+      <c r="S7" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>3</v>
+      </c>
+      <c r="U7" t="s">
+        <v>77</v>
+      </c>
+      <c r="V7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="33">
         <v>0.873702335795568</v>
       </c>
@@ -3545,8 +3561,41 @@
       <c r="J8" s="35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>0.87452585346376499</v>
+      </c>
+      <c r="M8">
+        <v>0.87592333799161504</v>
+      </c>
+      <c r="N8">
+        <v>0.99196446396486304</v>
+      </c>
+      <c r="O8">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P8">
+        <v>0.90829007785985205</v>
+      </c>
+      <c r="Q8">
+        <v>0.93232182072269898</v>
+      </c>
+      <c r="R8" t="s">
+        <v>70</v>
+      </c>
+      <c r="S8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>5</v>
+      </c>
+      <c r="U8" t="s">
+        <v>77</v>
+      </c>
+      <c r="V8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15" thickBot="1">
       <c r="A9" s="46">
         <v>0.877445597923737</v>
       </c>
@@ -3577,8 +3626,41 @@
       <c r="J9" s="48" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>0.87714613695348298</v>
+      </c>
+      <c r="M9">
+        <v>0.88058993811139896</v>
+      </c>
+      <c r="N9">
+        <v>0.99196446396486304</v>
+      </c>
+      <c r="O9">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P9">
+        <v>0.910161708923936</v>
+      </c>
+      <c r="Q9">
+        <v>0.93232182072269898</v>
+      </c>
+      <c r="R9" t="s">
+        <v>84</v>
+      </c>
+      <c r="S9" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>5</v>
+      </c>
+      <c r="U9" t="s">
+        <v>77</v>
+      </c>
+      <c r="V9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="30">
         <v>0.87183070473148305</v>
       </c>
@@ -3609,8 +3691,41 @@
       <c r="J10" s="32" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>0.87200538999999999</v>
+      </c>
+      <c r="M10">
+        <v>0.980535037</v>
+      </c>
+      <c r="N10">
+        <v>0.87088241200000005</v>
+      </c>
+      <c r="O10">
+        <v>0.93294569800000005</v>
+      </c>
+      <c r="P10">
+        <v>0.90669295299999997</v>
+      </c>
+      <c r="Q10">
+        <v>0.90464663599999995</v>
+      </c>
+      <c r="R10" t="s">
+        <v>70</v>
+      </c>
+      <c r="S10" t="b">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10" t="s">
+        <v>80</v>
+      </c>
+      <c r="V10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="33">
         <v>0.87542423637452504</v>
       </c>
@@ -3641,8 +3756,41 @@
       <c r="J11" s="35" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>0.87422639199999996</v>
+      </c>
+      <c r="M11">
+        <v>0.99565781600000003</v>
+      </c>
+      <c r="N11">
+        <v>0.87088241200000005</v>
+      </c>
+      <c r="O11">
+        <v>0.93294569800000005</v>
+      </c>
+      <c r="P11">
+        <v>0.90816530200000001</v>
+      </c>
+      <c r="Q11">
+        <v>0.90464663599999995</v>
+      </c>
+      <c r="R11" t="s">
+        <v>84</v>
+      </c>
+      <c r="S11" t="b">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11" t="s">
+        <v>80</v>
+      </c>
+      <c r="V11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="33">
         <v>0.87327809942104195</v>
       </c>
@@ -3673,8 +3821,41 @@
       <c r="J12" s="35" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>0.873702335795568</v>
+      </c>
+      <c r="M12">
+        <v>0.92401177879816299</v>
+      </c>
+      <c r="N12">
+        <v>0.91370533040527002</v>
+      </c>
+      <c r="O12">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P12">
+        <v>0.90941305649830295</v>
+      </c>
+      <c r="Q12">
+        <v>0.969729486923537</v>
+      </c>
+      <c r="R12" t="s">
+        <v>70</v>
+      </c>
+      <c r="S12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12" t="s">
+        <v>80</v>
+      </c>
+      <c r="V12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="33">
         <v>0.87714613695348298</v>
       </c>
@@ -3705,8 +3886,41 @@
       <c r="J13" s="35" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>0.87624775404272304</v>
+      </c>
+      <c r="M13">
+        <v>0.93047514473946802</v>
+      </c>
+      <c r="N13">
+        <v>0.91370533040527002</v>
+      </c>
+      <c r="O13">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P13">
+        <v>0.91115991215811498</v>
+      </c>
+      <c r="Q13">
+        <v>0.969729486923537</v>
+      </c>
+      <c r="R13" t="s">
+        <v>84</v>
+      </c>
+      <c r="S13" t="b">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13" t="s">
+        <v>80</v>
+      </c>
+      <c r="V13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="33">
         <v>0.87330305450189605</v>
       </c>
@@ -3737,8 +3951,41 @@
       <c r="J14" s="35" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>0.873702335795568</v>
+      </c>
+      <c r="M14">
+        <v>0.91031143940906301</v>
+      </c>
+      <c r="N14">
+        <v>0.92785486124975003</v>
+      </c>
+      <c r="O14">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P14">
+        <v>0.90941305649830295</v>
+      </c>
+      <c r="Q14">
+        <v>0.99026751846675898</v>
+      </c>
+      <c r="R14" t="s">
+        <v>70</v>
+      </c>
+      <c r="S14" t="b">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>3</v>
+      </c>
+      <c r="U14" t="s">
+        <v>80</v>
+      </c>
+      <c r="V14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="33">
         <v>0.87714613695348298</v>
       </c>
@@ -3769,8 +4016,41 @@
       <c r="J15" s="35" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>0.87622279896186805</v>
+      </c>
+      <c r="M15">
+        <v>0.91630065881413403</v>
+      </c>
+      <c r="N15">
+        <v>0.92785486124975003</v>
+      </c>
+      <c r="O15">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P15">
+        <v>0.91118486723896897</v>
+      </c>
+      <c r="Q15">
+        <v>0.99026751846675898</v>
+      </c>
+      <c r="R15" t="s">
+        <v>84</v>
+      </c>
+      <c r="S15" t="b">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>3</v>
+      </c>
+      <c r="U15" t="s">
+        <v>80</v>
+      </c>
+      <c r="V15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="33">
         <v>0.87327809942104195</v>
       </c>
@@ -3801,8 +4081,41 @@
       <c r="J16" s="35" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>0.87372729087642198</v>
+      </c>
+      <c r="M16">
+        <v>0.90799061688959803</v>
+      </c>
+      <c r="N16">
+        <v>0.92942703134358096</v>
+      </c>
+      <c r="O16">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P16">
+        <v>0.90943801157915705</v>
+      </c>
+      <c r="Q16">
+        <v>0.99223896985426197</v>
+      </c>
+      <c r="R16" t="s">
+        <v>70</v>
+      </c>
+      <c r="S16" t="b">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>5</v>
+      </c>
+      <c r="U16" t="s">
+        <v>80</v>
+      </c>
+      <c r="V16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="15" thickBot="1">
       <c r="A17" s="36">
         <v>0.87714613695348298</v>
       </c>
@@ -3833,9 +4146,42 @@
       <c r="J17" s="38" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>0.87624775404272304</v>
+      </c>
+      <c r="M17">
+        <v>0.91388001597125101</v>
+      </c>
+      <c r="N17">
+        <v>0.92942703134358096</v>
+      </c>
+      <c r="O17">
+        <v>0.93294569774406</v>
+      </c>
+      <c r="P17">
+        <v>0.91118486723896897</v>
+      </c>
+      <c r="Q17">
+        <v>0.99223896985426197</v>
+      </c>
+      <c r="R17" t="s">
+        <v>84</v>
+      </c>
+      <c r="S17" t="b">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>5</v>
+      </c>
+      <c r="U17" t="s">
+        <v>80</v>
+      </c>
+      <c r="V17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="15" thickBot="1"/>
+    <row r="19" spans="1:22">
       <c r="A19" s="30">
         <v>0.87195548013575497</v>
       </c>
@@ -3870,7 +4216,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22">
       <c r="A20" s="33">
         <v>0.87557396685965205</v>
       </c>
@@ -3902,7 +4248,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22">
       <c r="A21" s="33">
         <v>0.87365242563385903</v>
       </c>
@@ -3934,7 +4280,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="33">
         <v>0.87717109203433796</v>
       </c>
@@ -3966,7 +4312,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22">
       <c r="A23" s="33">
         <v>0.87372729087642198</v>
       </c>
@@ -3998,7 +4344,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22">
       <c r="A24" s="33">
         <v>0.87737073268117305</v>
       </c>
@@ -4030,7 +4376,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22">
       <c r="A25" s="33">
         <v>0.87372729087642198</v>
       </c>
@@ -4062,7 +4408,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="15" thickBot="1">
       <c r="A26" s="46">
         <v>0.877445597923737</v>
       </c>
@@ -4094,7 +4440,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22">
       <c r="A27" s="30">
         <v>0.87195548013575497</v>
       </c>
@@ -4126,7 +4472,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22">
       <c r="A28" s="33">
         <v>0.87557396685965205</v>
       </c>
@@ -4158,7 +4504,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22">
       <c r="A29" s="33">
         <v>0.87332800958275103</v>
       </c>
@@ -4190,7 +4536,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22">
       <c r="A30" s="33">
         <v>0.87689658614493904</v>
       </c>
@@ -4222,7 +4568,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22">
       <c r="A31" s="33">
         <v>0.87332800958275103</v>
       </c>
@@ -4254,7 +4600,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22">
       <c r="A32" s="33">
         <v>0.87707127171092003</v>
       </c>
@@ -4286,7 +4632,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="33">
         <v>0.87330305450189605</v>
       </c>
@@ -4318,7 +4664,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="15" thickBot="1">
       <c r="A34" s="36">
         <v>0.87707127171092003</v>
       </c>
@@ -4351,54 +4697,72 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J17">
-    <sortCondition ref="J2:J17"/>
-    <sortCondition ref="I2:I17"/>
+  <sortState ref="L2:V17">
+    <sortCondition ref="U2:U17"/>
+    <sortCondition ref="T2:T17"/>
+    <sortCondition ref="R2:R17"/>
   </sortState>
   <conditionalFormatting sqref="G2:G13">
-    <cfRule type="top10" dxfId="52" priority="32" rank="1"/>
+    <cfRule type="top10" dxfId="20" priority="32" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A17">
-    <cfRule type="top10" dxfId="43" priority="31" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="42" priority="37" rank="1"/>
+    <cfRule type="top10" dxfId="19" priority="31" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="18" priority="37" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="top10" dxfId="35" priority="17" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="34" priority="18" rank="1"/>
+    <cfRule type="top10" dxfId="17" priority="17" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="16" priority="18" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F17">
-    <cfRule type="top10" dxfId="33" priority="15" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="32" priority="16" rank="1"/>
+    <cfRule type="top10" dxfId="15" priority="15" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="14" priority="16" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:A34">
-    <cfRule type="top10" dxfId="29" priority="13" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="28" priority="14" rank="1"/>
+    <cfRule type="top10" dxfId="13" priority="13" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="12" priority="14" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:B34">
-    <cfRule type="top10" dxfId="25" priority="11" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="24" priority="12" rank="1"/>
+    <cfRule type="top10" dxfId="11" priority="11" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="10" priority="12" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:C34">
-    <cfRule type="top10" dxfId="21" priority="9" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="20" priority="10" rank="1"/>
+    <cfRule type="top10" dxfId="9" priority="9" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="8" priority="10" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19:E34">
-    <cfRule type="top10" dxfId="17" priority="7" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="16" priority="8" rank="1"/>
+    <cfRule type="top10" dxfId="7" priority="7" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="6" priority="8" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:F34">
-    <cfRule type="top10" dxfId="13" priority="5" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="12" priority="6" rank="1"/>
+    <cfRule type="top10" dxfId="5" priority="5" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="4" priority="6" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B17">
-    <cfRule type="top10" dxfId="7" priority="3" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="6" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="3" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="2" priority="4" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="top10" dxfId="3" priority="1" bottom="1" rank="1"/>
-    <cfRule type="top10" dxfId="2" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="0" priority="2" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>